<commit_message>
Replace Framework Version to "1"
</commit_message>
<xml_diff>
--- a/tools/excel/nist/sp-800-82/nist-sp-800-82-annex-f.xlsx
+++ b/tools/excel/nist/sp-800-82/nist-sp-800-82-annex-f.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\nist\sp-800-82\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687C8DD5-D3F4-469B-A52C-C40BD336F709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3859E5-4526-44A1-88FA-8A9D6C05E0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="444" yWindow="552" windowWidth="22140" windowHeight="13116" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="492" yWindow="588" windowWidth="22512" windowHeight="12264" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -4075,7 +4075,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4110,6 +4110,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4414,8 +4415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScale="157" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4444,8 +4445,8 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" s="14">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4609,8 +4610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A210" sqref="A210"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>